<commit_message>
release juni 2022: nieuwe wijkindelingen (+correcties)
Release notes
Nieuwe release gemeentegedragen wijken
- de bestaande nis7 wijken van Sint-Katelijne-Waver (closes #36) en Nieuwerkerken (closes #35) krijgen een naam vanuit de gemeente
- Closes #39: toevoegen wijkindelingen van Eeklo, Galmaarden, Halle, Harelbeke, Heusden-Zolder, Huldenberg, Ledegem, Mortsel, Oostrozebeke, Opwijk, Roosdaal, Sint-Katelijne-Waver, Wemmel, Wielsbeke, Zedelgem, Zele

Kleine andere aanpassingen:
- aanpassing naam van één statsec op vraag van gemeentebestuur (closes #38)
- deelgemeente2019 laten verdwijnen (niet meer relevant, en was kapot) (closes #41)
- correctie naam van een Eerstelijnszone (ELZ) op vraag van die ELZ zelf) (closes #34)
</commit_message>
<xml_diff>
--- a/data_voor_swing/gebiedsdefinities/elz.xlsx
+++ b/data_voor_swing/gebiedsdefinities/elz.xlsx
@@ -656,17 +656,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>elz46</t>
+          <t>elz14</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hageland</t>
+          <t>Haspengouw</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hageland</t>
+          <t>Haspengouw</t>
         </is>
       </c>
     </row>
@@ -676,17 +676,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>elz14</t>
+          <t>elz15</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Haspengouw</t>
+          <t>Herkenrode</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Haspengouw</t>
+          <t>Herkenrode</t>
         </is>
       </c>
     </row>
@@ -696,17 +696,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>elz15</t>
+          <t>elz16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Herkenrode</t>
+          <t>Houtland en Polder</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Herkenrode</t>
+          <t>Houtland en Polder</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>elz16</t>
+          <t>elz12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Houtland en Polder</t>
+          <t>Kemp en Duin</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Houtland en Polder</t>
+          <t>Kemp en Duin</t>
         </is>
       </c>
     </row>
@@ -736,17 +736,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>elz12</t>
+          <t>elz41</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Kemp en Duin</t>
+          <t>Kempenland</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kemp en Duin</t>
+          <t>Kempenland</t>
         </is>
       </c>
     </row>
@@ -756,17 +756,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>elz41</t>
+          <t>elz17</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Kempenland</t>
+          <t>Klein-Brabant Vaartland</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Kempenland</t>
+          <t>Klein-Brabant Vaartland</t>
         </is>
       </c>
     </row>
@@ -776,17 +776,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>elz17</t>
+          <t>elz19</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Klein-Brabant Vaartland</t>
+          <t>Leuven</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Klein-Brabant Vaartland</t>
+          <t>Leuven</t>
         </is>
       </c>
     </row>
@@ -796,17 +796,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>elz19</t>
+          <t>elz20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Leuven</t>
+          <t>Leuven Noord</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Leuven</t>
+          <t>Leuven Noord</t>
         </is>
       </c>
     </row>
@@ -816,17 +816,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>elz20</t>
+          <t>elz21</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Leuven Noord</t>
+          <t>Leuven Zuid</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Leuven Noord</t>
+          <t>Leuven Zuid</t>
         </is>
       </c>
     </row>
@@ -836,17 +836,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>elz21</t>
+          <t>elz22</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Leuven Zuid</t>
+          <t>Maasland</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Leuven Zuid</t>
+          <t>Maasland</t>
         </is>
       </c>
     </row>
@@ -856,17 +856,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>elz22</t>
+          <t>elz23</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Maasland</t>
+          <t>Mechelen-Katelijne</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Maasland</t>
+          <t>Mechelen-Katelijne</t>
         </is>
       </c>
     </row>
@@ -876,17 +876,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>elz23</t>
+          <t>elz39</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Mechelen-Katelijne</t>
+          <t>Midden WVL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Mechelen-Katelijne</t>
+          <t>Midden WVL</t>
         </is>
       </c>
     </row>
@@ -896,17 +896,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>elz39</t>
+          <t>elz25</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Midden WVL</t>
+          <t>Middenkempen</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Midden WVL</t>
+          <t>Middenkempen</t>
         </is>
       </c>
     </row>
@@ -916,17 +916,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>elz25</t>
+          <t>elz26</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Middenkempen</t>
+          <t>MidWestLim</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Middenkempen</t>
+          <t>MidWestLim</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>elz26</t>
+          <t>elz29</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MidWestLim</t>
+          <t>N-O-Waasland</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>MidWestLim</t>
+          <t>N-O-Waasland</t>
         </is>
       </c>
     </row>
@@ -956,17 +956,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>elz29</t>
+          <t>elz28</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>N-O-Waasland</t>
+          <t>Noord-Limburg</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>N-O-Waasland</t>
+          <t>Noord-Limburg</t>
         </is>
       </c>
     </row>
@@ -976,17 +976,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>elz28</t>
+          <t>elz27</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Noord-Limburg</t>
+          <t>Noorderkempen</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Noord-Limburg</t>
+          <t>Noorderkempen</t>
         </is>
       </c>
     </row>
@@ -996,17 +996,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>elz27</t>
+          <t>elz32</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Noorderkempen</t>
+          <t>Oost-Meetjesland</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Noorderkempen</t>
+          <t>Oost-Meetjesland</t>
         </is>
       </c>
     </row>
@@ -1016,17 +1016,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>elz32</t>
+          <t>elz30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Oost-Meetjesland</t>
+          <t>Oostende-Bredene</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Oost-Meetjesland</t>
+          <t>Oostende-Bredene</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>elz30</t>
+          <t>elz31</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Oostende-Bredene</t>
+          <t>Oostkust</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Oostende-Bredene</t>
+          <t>Oostkust</t>
         </is>
       </c>
     </row>
@@ -1056,17 +1056,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>elz31</t>
+          <t>elz33</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Oostkust</t>
+          <t>Pajottenland</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Oostkust</t>
+          <t>Pajottenland</t>
         </is>
       </c>
     </row>
@@ -1076,17 +1076,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>elz33</t>
+          <t>elz34</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Pajottenland</t>
+          <t>Pallieterland</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Pajottenland</t>
+          <t>Pallieterland</t>
         </is>
       </c>
     </row>
@@ -1096,17 +1096,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>elz34</t>
+          <t>elz35</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Pallieterland</t>
+          <t>Panacea</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pallieterland</t>
+          <t>Panacea</t>
         </is>
       </c>
     </row>
@@ -1116,17 +1116,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>elz35</t>
+          <t>elz36</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Panacea</t>
+          <t>Regio Aalst</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Panacea</t>
+          <t>Regio Aalst</t>
         </is>
       </c>
     </row>
@@ -1136,17 +1136,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>elz36</t>
+          <t>elz37</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Regio Aalst</t>
+          <t>Regio Grimbergen</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Regio Aalst</t>
+          <t>Regio Grimbergen</t>
         </is>
       </c>
     </row>
@@ -1156,17 +1156,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>elz37</t>
+          <t>elz18</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Regio Grimbergen</t>
+          <t>Regio Kortrijk</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Regio Grimbergen</t>
+          <t>Regio Kortrijk</t>
         </is>
       </c>
     </row>
@@ -1176,17 +1176,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>elz18</t>
+          <t>elz24</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Regio Kortrijk</t>
+          <t>Regio Menen</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Regio Kortrijk</t>
+          <t>Regio Menen</t>
         </is>
       </c>
     </row>
@@ -1196,17 +1196,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>elz24</t>
+          <t>elz50</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Regio Menen</t>
+          <t>Regio Waregem</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Regio Menen</t>
+          <t>Regio Waregem</t>
         </is>
       </c>
     </row>
@@ -1216,17 +1216,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>elz50</t>
+          <t>elz40</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Regio Waregem</t>
+          <t>RITS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Regio Waregem</t>
+          <t>RITS</t>
         </is>
       </c>
     </row>
@@ -1236,17 +1236,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>elz40</t>
+          <t>elz43</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RITS</t>
+          <t>RupeLaar</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>RITS</t>
+          <t>RupeLaar</t>
         </is>
       </c>
     </row>
@@ -1256,17 +1256,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>elz43</t>
+          <t>elz44</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RupeLaar</t>
+          <t>Schelde en Leie</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>RupeLaar</t>
+          <t>Schelde en Leie</t>
         </is>
       </c>
     </row>
@@ -1276,17 +1276,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>elz44</t>
+          <t>elz45</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Schelde en Leie</t>
+          <t>Scheldekracht</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Schelde en Leie</t>
+          <t>Scheldekracht</t>
         </is>
       </c>
     </row>
@@ -1296,17 +1296,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>elz45</t>
+          <t>elz48</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Scheldekracht</t>
+          <t>Vlaamse Ardennen</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Scheldekracht</t>
+          <t>Vlaamse Ardennen</t>
         </is>
       </c>
     </row>
@@ -1316,17 +1316,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>elz48</t>
+          <t>elz49</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vlaamse Ardennen</t>
+          <t>Voorkempen</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Vlaamse Ardennen</t>
+          <t>Voorkempen</t>
         </is>
       </c>
     </row>
@@ -1336,17 +1336,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>elz49</t>
+          <t>elz4</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Voorkempen</t>
+          <t>WE40</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Voorkempen</t>
+          <t>WE40</t>
         </is>
       </c>
     </row>
@@ -1356,17 +1356,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>elz4</t>
+          <t>elz51</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>WE40</t>
+          <t>West-Limburg</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>WE40</t>
+          <t>West-Limburg</t>
         </is>
       </c>
     </row>
@@ -1376,17 +1376,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>elz51</t>
+          <t>elz52</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>West-Limburg</t>
+          <t>West-Meetjesland</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>West-Limburg</t>
+          <t>West-Meetjesland</t>
         </is>
       </c>
     </row>
@@ -1396,17 +1396,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>elz52</t>
+          <t>elz38</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>West-Meetjesland</t>
+          <t>Westhoek</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>West-Meetjesland</t>
+          <t>Westhoek</t>
         </is>
       </c>
     </row>
@@ -1416,17 +1416,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>elz38</t>
+          <t>elz47</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Westhoek</t>
+          <t>Westkust&amp;Polder</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Westhoek</t>
+          <t>Westkust&amp;Polder</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>elz47</t>
+          <t>elz57</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Westkust&amp;Polder</t>
+          <t>Z-W-Waasland</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Westkust&amp;Polder</t>
+          <t>Z-W-Waasland</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>elz57</t>
+          <t>elz53</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Z-W-Waasland</t>
+          <t>Zennevallei</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Z-W-Waasland</t>
+          <t>Zennevallei</t>
         </is>
       </c>
     </row>
@@ -1476,17 +1476,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>elz53</t>
+          <t>elz54</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Zennevallei</t>
+          <t>ZOLim</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Zennevallei</t>
+          <t>ZOLim</t>
         </is>
       </c>
     </row>
@@ -1496,17 +1496,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>elz54</t>
+          <t>elz55</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ZOLim</t>
+          <t>ZORA</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ZOLim</t>
+          <t>ZORA</t>
         </is>
       </c>
     </row>
@@ -1516,17 +1516,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>elz55</t>
+          <t>elz56</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ZORA</t>
+          <t>Zuiderkempen</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ZORA</t>
+          <t>Zuiderkempen</t>
         </is>
       </c>
     </row>
@@ -1536,17 +1536,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>elz56</t>
+          <t>elz46</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Zuiderkempen</t>
+          <t>Zuidoost Hageland</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Zuiderkempen</t>
+          <t>Zuidoost Hageland</t>
         </is>
       </c>
     </row>
@@ -1561,12 +1561,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend</t>
+          <t>ELZ onbekend</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend</t>
+          <t>ELZ onbekend</t>
         </is>
       </c>
     </row>
@@ -1581,12 +1581,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend (Brussel)</t>
+          <t>ELZ onbekend (Brussel)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend (Brussel)</t>
+          <t>ELZ onbekend (Brussel)</t>
         </is>
       </c>
     </row>
@@ -1601,12 +1601,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend (Vlaanderen)</t>
+          <t>ELZ onbekend (Vlaanderen)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Eerstelijnszone onbekend (Vlaanderen)</t>
+          <t>ELZ onbekend (Vlaanderen)</t>
         </is>
       </c>
     </row>

</xml_diff>